<commit_message>
update at end semester
</commit_message>
<xml_diff>
--- a/Time Tracking/Francesco Time Tracking-P.I.E..xlsx
+++ b/Time Tracking/Francesco Time Tracking-P.I.E..xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescolimoni/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43C885E-36F0-BD42-882B-34A9BDB12017}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C88A97-8CB2-5744-A8FD-2C7B64B11D73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -130,6 +130,33 @@
   </si>
   <si>
     <t xml:space="preserve">Testing </t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Sprint 6</t>
+  </si>
+  <si>
+    <t>connected classes between them</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debuggin and reasearching </t>
+  </si>
+  <si>
+    <t>changed the integration between the classes</t>
+  </si>
+  <si>
+    <t>changed the design or layer class with a fixed number  of layers (5)</t>
+  </si>
+  <si>
+    <t>TOTAL SEMESTER  HOURS</t>
+  </si>
+  <si>
+    <t>Redesigned the component of the layer class</t>
   </si>
 </sst>
 </file>
@@ -177,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -186,6 +213,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -507,10 +535,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -520,11 +548,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -651,11 +679,11 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
@@ -722,11 +750,11 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
@@ -792,11 +820,242 @@
         <v>10</v>
       </c>
     </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="2">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="4">
+        <f>B47</f>
+        <v>8</v>
+      </c>
+      <c r="C38" s="4"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="2">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="4">
+        <f>B42+B43+B44+B45</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="2">
+        <v>4</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="2">
+        <v>2</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="2">
+        <v>4</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56">
+        <f>B51+B52+B53+B54</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57">
+        <f>B13+B21+B29+B38+B47+B56</f>
+        <v>62.5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A49:C49"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A40:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>